<commit_message>
Changes made across the board
I had to merge a couple of steps because a large file >100Mb was added by mistake in one of the steps.
</commit_message>
<xml_diff>
--- a/SATIM/DataSpreadsheets/ExchangeRate_Currency_Deflator_v00.xlsx
+++ b/SATIM/DataSpreadsheets/ExchangeRate_Currency_Deflator_v00.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE\SATIM\DataSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD7BB8E-A509-471F-AD4B-38DD139A006A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA3800B-9184-4C5C-9CE4-BF9D83F9FE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3615" yWindow="-21210" windowWidth="28770" windowHeight="15570" xr2:uid="{229B7DCB-2FD0-4685-ABA3-BD548D839EC5}"/>
+    <workbookView xWindow="8115" yWindow="-15600" windowWidth="25275" windowHeight="14745" xr2:uid="{229B7DCB-2FD0-4685-ABA3-BD548D839EC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Calcs" sheetId="1" r:id="rId1"/>
     <sheet name="Readme" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -503,7 +503,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -607,6 +607,7 @@
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -6926,10 +6927,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F9E0C6-CEFF-47DC-AC13-AB5365841E40}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="C2:AE153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6953,7 +6955,7 @@
         <v>29</v>
       </c>
       <c r="E3" s="29">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="O3" t="s">
         <v>0</v>
@@ -7015,57 +7017,57 @@
         <v>33</v>
       </c>
       <c r="E4" s="29">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="O4" t="s">
         <v>1</v>
       </c>
       <c r="P4" s="13">
-        <f>SUMIF($C$18:$C$153,P$3,$E$18:$E$153)/COUNTIF($C$18:$C$153,P$3)</f>
+        <f t="shared" ref="P4:AA4" si="1">SUMIF($C$18:$C$153,P$3,$E$18:$E$153)/COUNTIF($C$18:$C$153,P$3)</f>
         <v>7.3112916666666665</v>
       </c>
       <c r="Q4" s="13">
-        <f>SUMIF($C$18:$C$153,Q$3,$E$18:$E$153)/COUNTIF($C$18:$C$153,Q$3)</f>
+        <f t="shared" si="1"/>
         <v>7.2519583333333335</v>
       </c>
       <c r="R4" s="13">
-        <f>SUMIF($C$18:$C$153,R$3,$E$18:$E$153)/COUNTIF($C$18:$C$153,R$3)</f>
+        <f t="shared" si="1"/>
         <v>8.2029916666666658</v>
       </c>
       <c r="S4" s="13">
-        <f>SUMIF($C$18:$C$153,S$3,$E$18:$E$153)/COUNTIF($C$18:$C$153,S$3)</f>
+        <f t="shared" si="1"/>
         <v>9.7545999999999999</v>
       </c>
       <c r="T4" s="13">
-        <f>SUMIF($C$18:$C$153,T$3,$E$18:$E$153)/COUNTIF($C$18:$C$153,T$3)</f>
+        <f t="shared" si="1"/>
         <v>10.874366666666667</v>
       </c>
       <c r="U4" s="13">
-        <f>SUMIF($C$18:$C$153,U$3,$E$18:$E$153)/COUNTIF($C$18:$C$153,U$3)</f>
+        <f t="shared" si="1"/>
         <v>12.937225000000003</v>
       </c>
       <c r="V4" s="13">
-        <f>SUMIF($C$18:$C$153,V$3,$E$18:$E$153)/COUNTIF($C$18:$C$153,V$3)</f>
+        <f t="shared" si="1"/>
         <v>14.569299999999998</v>
       </c>
       <c r="W4" s="13">
-        <f>SUMIF($C$18:$C$153,W$3,$E$18:$E$153)/COUNTIF($C$18:$C$153,W$3)</f>
+        <f t="shared" si="1"/>
         <v>13.292041666666664</v>
       </c>
       <c r="X4" s="13">
-        <f>SUMIF($C$18:$C$153,X$3,$E$18:$E$153)/COUNTIF($C$18:$C$153,X$3)</f>
+        <f t="shared" si="1"/>
         <v>13.294000000000002</v>
       </c>
       <c r="Y4" s="13">
-        <f>SUMIF($C$18:$C$153,Y$3,$E$18:$E$153)/COUNTIF($C$18:$C$153,Y$3)</f>
+        <f t="shared" si="1"/>
         <v>14.435708333333336</v>
       </c>
       <c r="Z4" s="13">
-        <f>SUMIF($C$18:$C$153,Z$3,$E$18:$E$153)/COUNTIF($C$18:$C$153,Z$3)</f>
+        <f t="shared" si="1"/>
         <v>16.584166666666668</v>
       </c>
       <c r="AA4" s="32">
-        <f>SUMIF($C$18:$C$153,AA$3,$E$18:$E$153)/COUNTIF($C$18:$C$153,AA$3)</f>
+        <f t="shared" si="1"/>
         <v>14.890974999999999</v>
       </c>
     </row>
@@ -7107,8 +7109,7 @@
         <v>1.6393210749646394</v>
       </c>
       <c r="AA5" s="31">
-        <f>Z5/Y5*Z5</f>
-        <v>1.6933806826060758</v>
+        <v>1.7070000000000001</v>
       </c>
       <c r="AC5" t="s">
         <v>28</v>
@@ -7117,15 +7118,15 @@
     <row r="6" spans="3:29">
       <c r="D6" s="30" t="str">
         <f>"1 "&amp;E3&amp;" ZAR = "</f>
-        <v xml:space="preserve">1 2020 ZAR = </v>
+        <v xml:space="preserve">1 2015 ZAR = </v>
       </c>
       <c r="E6" s="33">
         <f>INDEX($P$5:$AB$5,1,MATCH($E$4,$P$3:$AB$3,0))/INDEX($P$5:$AB$5,1,MATCH($E$3,$P$3:$AB$3,0))</f>
-        <v>0.79378774805867114</v>
+        <v>1.3117923913043481</v>
       </c>
       <c r="F6" t="str">
         <f>E4&amp;" ZAR"</f>
-        <v>2015 ZAR</v>
+        <v>2021 ZAR</v>
       </c>
       <c r="O6" t="s">
         <v>11</v>
@@ -7171,15 +7172,19 @@
     <row r="7" spans="3:29">
       <c r="D7" s="30" t="str">
         <f>"1 "&amp;E3&amp;" USD = "</f>
-        <v xml:space="preserve">1 2020 USD = </v>
+        <v xml:space="preserve">1 2015 USD = </v>
       </c>
       <c r="E7" s="33">
         <f>INDEX($P$6:$AB$6,1,MATCH($E$4,$P$3:$AB$3,0))/INDEX($P$6:$AB$6,1,MATCH($E$3,$P$3:$AB$3,0))</f>
-        <v>0.91579183265008068</v>
+        <v>1.1054224397384176</v>
       </c>
       <c r="F7" t="str">
         <f>E4&amp;" USD"</f>
-        <v>2015 USD</v>
+        <v>2021 USD</v>
+      </c>
+      <c r="AA7" s="39">
+        <f>AA5/U5</f>
+        <v>1.3117923913043481</v>
       </c>
     </row>
     <row r="8" spans="3:29">
@@ -7199,70 +7204,70 @@
       </c>
       <c r="D9" s="30" t="str">
         <f>"1 "&amp;E3&amp;" USD = "</f>
-        <v xml:space="preserve">1 2020 USD = </v>
+        <v xml:space="preserve">1 2015 USD = </v>
       </c>
       <c r="E9">
         <f>INDEX($P$4:$AB$4,1,MATCH($E$3,$P$3:$AB$3,0))</f>
-        <v>16.584166666666668</v>
+        <v>12.937225000000003</v>
       </c>
       <c r="F9" t="str">
         <f>E3&amp;" ZAR = "</f>
-        <v xml:space="preserve">2020 ZAR = </v>
+        <v xml:space="preserve">2015 ZAR = </v>
       </c>
       <c r="G9" s="33">
         <f>E9*E6</f>
-        <v>13.164308311763014</v>
+        <v>16.9709533195924</v>
       </c>
       <c r="H9" t="str">
         <f>E4&amp;" ZAR"</f>
-        <v>2015 ZAR</v>
+        <v>2021 ZAR</v>
       </c>
       <c r="P9">
         <f>P3</f>
         <v>2010</v>
       </c>
       <c r="Q9">
-        <f t="shared" ref="Q9:AA9" si="1">Q3</f>
+        <f t="shared" ref="Q9:AA9" si="2">Q3</f>
         <v>2011</v>
       </c>
       <c r="R9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2012</v>
       </c>
       <c r="S9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2013</v>
       </c>
       <c r="T9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2014</v>
       </c>
       <c r="U9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2015</v>
       </c>
       <c r="V9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2016</v>
       </c>
       <c r="W9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2017</v>
       </c>
       <c r="X9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2018</v>
       </c>
       <c r="Y9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2019</v>
       </c>
       <c r="Z9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2020</v>
       </c>
       <c r="AA9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2021</v>
       </c>
     </row>
@@ -7272,23 +7277,23 @@
       </c>
       <c r="D10" s="30" t="str">
         <f>"1 "&amp;E3&amp;" USD = "</f>
-        <v xml:space="preserve">1 2020 USD = </v>
+        <v xml:space="preserve">1 2015 USD = </v>
       </c>
       <c r="E10">
         <f>E7</f>
-        <v>0.91579183265008068</v>
+        <v>1.1054224397384176</v>
       </c>
       <c r="F10" t="str">
         <f>E4&amp;" USD = "</f>
-        <v xml:space="preserve">2015 USD = </v>
+        <v xml:space="preserve">2021 USD = </v>
       </c>
       <c r="G10" s="33">
         <f>INDEX($P$4:$AB$4,1,MATCH($E$4,$P$3:$AB$3,0))*E10</f>
-        <v>11.847804992156442</v>
+        <v>16.460817914583782</v>
       </c>
       <c r="H10" t="str">
         <f>E4&amp;" ZAR"</f>
-        <v>2015 ZAR</v>
+        <v>2021 ZAR</v>
       </c>
       <c r="O10" t="s">
         <v>30</v>
@@ -7336,15 +7341,15 @@
       </c>
       <c r="D11" s="30" t="str">
         <f>D10</f>
-        <v xml:space="preserve">1 2020 USD = </v>
+        <v xml:space="preserve">1 2015 USD = </v>
       </c>
       <c r="G11" s="33">
         <f>AVERAGE(G9:G10)</f>
-        <v>12.506056651959728</v>
+        <v>16.715885617088091</v>
       </c>
       <c r="H11" t="str">
         <f>H10</f>
-        <v>2015 ZAR</v>
+        <v>2021 ZAR</v>
       </c>
       <c r="O11" t="s">
         <v>31</v>
@@ -7436,47 +7441,47 @@
         <v>3.2160570827086965</v>
       </c>
       <c r="Q13">
-        <f t="shared" ref="Q13:AA13" si="2">_xlfn.STDEV.S(Q10:Q11)</f>
+        <f t="shared" ref="Q13:AA13" si="3">_xlfn.STDEV.S(Q10:Q11)</f>
         <v>3.2811431314775441</v>
       </c>
       <c r="R13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.637182041113026</v>
       </c>
       <c r="S13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.6527390944341185</v>
       </c>
       <c r="T13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1200041916100147</v>
       </c>
       <c r="U13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.65375482899360748</v>
       </c>
       <c r="W13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.44978474269419172</v>
       </c>
       <c r="X13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.60846814498108848</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.11115951829690279</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.93090842474840729</v>
       </c>
       <c r="AA13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.11362120409528452</v>
       </c>
     </row>
@@ -7487,51 +7492,51 @@
     </row>
     <row r="15" spans="3:29">
       <c r="P15">
-        <f t="shared" ref="P15:AA15" si="3">P3</f>
+        <f t="shared" ref="P15:AA15" si="4">P3</f>
         <v>2010</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2011</v>
       </c>
       <c r="R15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2012</v>
       </c>
       <c r="S15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2013</v>
       </c>
       <c r="T15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2014</v>
       </c>
       <c r="U15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2015</v>
       </c>
       <c r="V15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2016</v>
       </c>
       <c r="W15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2017</v>
       </c>
       <c r="X15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2018</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2019</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2020</v>
       </c>
       <c r="AA15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2021</v>
       </c>
     </row>
@@ -7643,7 +7648,7 @@
     </row>
     <row r="18" spans="3:27" ht="18" thickBot="1">
       <c r="C18">
-        <f t="shared" ref="C18:C20" si="4">YEAR(D18)</f>
+        <f t="shared" ref="C18:C20" si="5">YEAR(D18)</f>
         <v>2021</v>
       </c>
       <c r="D18" s="34">
@@ -7709,7 +7714,7 @@
     </row>
     <row r="19" spans="3:27" ht="18" thickBot="1">
       <c r="C19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2021</v>
       </c>
       <c r="D19" s="3">
@@ -7737,57 +7742,57 @@
         <v>40</v>
       </c>
       <c r="P19">
-        <f>_xlfn.STDEV.S(P16:P17)</f>
+        <f t="shared" ref="P19:AA19" si="6">_xlfn.STDEV.S(P16:P17)</f>
         <v>4.185164652737253</v>
       </c>
       <c r="Q19">
-        <f>_xlfn.STDEV.S(Q16:Q17)</f>
+        <f t="shared" si="6"/>
         <v>4.2309631463451218</v>
       </c>
       <c r="R19">
-        <f>_xlfn.STDEV.S(R16:R17)</f>
+        <f t="shared" si="6"/>
         <v>3.5311317301022185</v>
       </c>
       <c r="S19">
-        <f>_xlfn.STDEV.S(S16:S17)</f>
+        <f t="shared" si="6"/>
         <v>2.4737781153349752</v>
       </c>
       <c r="T19">
-        <f>_xlfn.STDEV.S(T16:T17)</f>
+        <f t="shared" si="6"/>
         <v>1.895831350679628</v>
       </c>
       <c r="U19">
-        <f>_xlfn.STDEV.S(U16:U17)</f>
+        <f t="shared" si="6"/>
         <v>0.70397679683353465</v>
       </c>
       <c r="V19">
-        <f>_xlfn.STDEV.S(V16:V17)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="W19">
-        <f>_xlfn.STDEV.S(W16:W17)</f>
+        <f t="shared" si="6"/>
         <v>1.1590089429360562</v>
       </c>
       <c r="X19">
-        <f>_xlfn.STDEV.S(X16:X17)</f>
+        <f t="shared" si="6"/>
         <v>1.3115241286944341</v>
       </c>
       <c r="Y19">
-        <f>_xlfn.STDEV.S(Y16:Y17)</f>
+        <f t="shared" si="6"/>
         <v>0.77085739220562444</v>
       </c>
       <c r="Z19">
-        <f>_xlfn.STDEV.S(Z16:Z17)</f>
+        <f t="shared" si="6"/>
         <v>0.34523721453271761</v>
       </c>
       <c r="AA19">
-        <f>_xlfn.STDEV.S(AA16:AA17)</f>
+        <f t="shared" si="6"/>
         <v>0.7576650583979172</v>
       </c>
     </row>
     <row r="20" spans="3:27" ht="18" thickBot="1">
       <c r="C20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2021</v>
       </c>
       <c r="D20" s="3">
@@ -7817,7 +7822,7 @@
     </row>
     <row r="21" spans="3:27" ht="18" thickBot="1">
       <c r="C21">
-        <f t="shared" ref="C21:C83" si="5">YEAR(D21)</f>
+        <f t="shared" ref="C21:C83" si="7">YEAR(D21)</f>
         <v>2021</v>
       </c>
       <c r="D21" s="3">
@@ -7842,57 +7847,57 @@
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="P21">
-        <f>P9</f>
+        <f t="shared" ref="P21:AA21" si="8">P9</f>
         <v>2010</v>
       </c>
       <c r="Q21">
-        <f>Q9</f>
+        <f t="shared" si="8"/>
         <v>2011</v>
       </c>
       <c r="R21">
-        <f>R9</f>
+        <f t="shared" si="8"/>
         <v>2012</v>
       </c>
       <c r="S21">
-        <f>S9</f>
+        <f t="shared" si="8"/>
         <v>2013</v>
       </c>
       <c r="T21">
-        <f>T9</f>
+        <f t="shared" si="8"/>
         <v>2014</v>
       </c>
       <c r="U21">
-        <f>U9</f>
+        <f t="shared" si="8"/>
         <v>2015</v>
       </c>
       <c r="V21">
-        <f>V9</f>
+        <f t="shared" si="8"/>
         <v>2016</v>
       </c>
       <c r="W21">
-        <f>W9</f>
+        <f t="shared" si="8"/>
         <v>2017</v>
       </c>
       <c r="X21">
-        <f>X9</f>
+        <f t="shared" si="8"/>
         <v>2018</v>
       </c>
       <c r="Y21">
-        <f>Y9</f>
+        <f t="shared" si="8"/>
         <v>2019</v>
       </c>
       <c r="Z21">
-        <f>Z9</f>
+        <f t="shared" si="8"/>
         <v>2020</v>
       </c>
       <c r="AA21">
-        <f>AA9</f>
+        <f t="shared" si="8"/>
         <v>2021</v>
       </c>
     </row>
     <row r="22" spans="3:27" ht="18" thickBot="1">
       <c r="C22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2020</v>
       </c>
       <c r="D22" s="3">
@@ -7958,7 +7963,7 @@
     </row>
     <row r="23" spans="3:27" ht="18" thickBot="1">
       <c r="C23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2020</v>
       </c>
       <c r="D23" s="3">
@@ -8024,7 +8029,7 @@
     </row>
     <row r="24" spans="3:27" ht="18" thickBot="1">
       <c r="C24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2020</v>
       </c>
       <c r="D24" s="3">
@@ -8090,7 +8095,7 @@
     </row>
     <row r="25" spans="3:27" ht="18" thickBot="1">
       <c r="C25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2020</v>
       </c>
       <c r="D25" s="3">
@@ -8122,53 +8127,53 @@
         <v>3.7632483819341918</v>
       </c>
       <c r="Q25">
-        <f t="shared" ref="Q25:AA25" si="6">_xlfn.STDEV.S(Q22:Q23)</f>
+        <f t="shared" ref="Q25:AA25" si="9">_xlfn.STDEV.S(Q22:Q23)</f>
         <v>3.8474886238714787</v>
       </c>
       <c r="R25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>3.0652600244846093</v>
       </c>
       <c r="S25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.8668468625190691</v>
       </c>
       <c r="T25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.2195168096929787</v>
       </c>
       <c r="U25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.14622777683474844</v>
       </c>
       <c r="V25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.94170272572350489</v>
       </c>
       <c r="W25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.40714794294846046</v>
       </c>
       <c r="X25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0.60404387414729122</v>
       </c>
       <c r="Y25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Z25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1.2692177391315271</v>
       </c>
       <c r="AA25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>6.2862100545342985E-3</v>
       </c>
     </row>
     <row r="26" spans="3:27" ht="18" thickBot="1">
       <c r="C26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2020</v>
       </c>
       <c r="D26" s="3">
@@ -8195,7 +8200,7 @@
     </row>
     <row r="27" spans="3:27" ht="18" thickBot="1">
       <c r="C27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2020</v>
       </c>
       <c r="D27" s="3">
@@ -8222,7 +8227,7 @@
     </row>
     <row r="28" spans="3:27" ht="18" thickBot="1">
       <c r="C28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2020</v>
       </c>
       <c r="D28" s="3">
@@ -8249,7 +8254,7 @@
     </row>
     <row r="29" spans="3:27" ht="18" thickBot="1">
       <c r="C29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2020</v>
       </c>
       <c r="D29" s="3">
@@ -8276,7 +8281,7 @@
     </row>
     <row r="30" spans="3:27" ht="18" thickBot="1">
       <c r="C30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2020</v>
       </c>
       <c r="D30" s="3">
@@ -8303,7 +8308,7 @@
     </row>
     <row r="31" spans="3:27" ht="18" thickBot="1">
       <c r="C31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2020</v>
       </c>
       <c r="D31" s="3">
@@ -8330,7 +8335,7 @@
     </row>
     <row r="32" spans="3:27" ht="18" thickBot="1">
       <c r="C32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2020</v>
       </c>
       <c r="D32" s="3">
@@ -8357,7 +8362,7 @@
     </row>
     <row r="33" spans="3:31" ht="18" thickBot="1">
       <c r="C33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2020</v>
       </c>
       <c r="D33" s="3">
@@ -8384,7 +8389,7 @@
     </row>
     <row r="34" spans="3:31" ht="18" thickBot="1">
       <c r="C34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2019</v>
       </c>
       <c r="D34" s="3">
@@ -8411,7 +8416,7 @@
     </row>
     <row r="35" spans="3:31" ht="18" thickBot="1">
       <c r="C35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2019</v>
       </c>
       <c r="D35" s="3">
@@ -8438,7 +8443,7 @@
     </row>
     <row r="36" spans="3:31" ht="18" thickBot="1">
       <c r="C36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2019</v>
       </c>
       <c r="D36" s="3">
@@ -8465,7 +8470,7 @@
     </row>
     <row r="37" spans="3:31" ht="18" thickBot="1">
       <c r="C37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2019</v>
       </c>
       <c r="D37" s="3">
@@ -8492,7 +8497,7 @@
     </row>
     <row r="38" spans="3:31" ht="18" thickBot="1">
       <c r="C38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2019</v>
       </c>
       <c r="D38" s="3">
@@ -8519,7 +8524,7 @@
     </row>
     <row r="39" spans="3:31" ht="18" thickBot="1">
       <c r="C39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2019</v>
       </c>
       <c r="D39" s="3">
@@ -8546,7 +8551,7 @@
     </row>
     <row r="40" spans="3:31" ht="18" thickBot="1">
       <c r="C40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2019</v>
       </c>
       <c r="D40" s="3">
@@ -8573,7 +8578,7 @@
     </row>
     <row r="41" spans="3:31" ht="18" thickBot="1">
       <c r="C41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2019</v>
       </c>
       <c r="D41" s="3">
@@ -8600,7 +8605,7 @@
     </row>
     <row r="42" spans="3:31" ht="18" thickBot="1">
       <c r="C42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2019</v>
       </c>
       <c r="D42" s="3">
@@ -8627,7 +8632,7 @@
     </row>
     <row r="43" spans="3:31" ht="18" thickBot="1">
       <c r="C43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2019</v>
       </c>
       <c r="D43" s="3">
@@ -8657,7 +8662,7 @@
     </row>
     <row r="44" spans="3:31" ht="18" thickBot="1">
       <c r="C44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2019</v>
       </c>
       <c r="D44" s="3">
@@ -8732,7 +8737,7 @@
     </row>
     <row r="45" spans="3:31" ht="18" thickBot="1">
       <c r="C45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2019</v>
       </c>
       <c r="D45" s="3">
@@ -8805,13 +8810,13 @@
         <v>1.6</v>
       </c>
       <c r="AE45">
-        <f t="shared" ref="AE45:AE55" si="7">AB45/$AB$45</f>
+        <f t="shared" ref="AE45:AE55" si="10">AB45/$AB$45</f>
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="3:31" ht="18" thickBot="1">
       <c r="C46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2018</v>
       </c>
       <c r="D46" s="3">
@@ -8884,13 +8889,13 @@
         <v>3.2</v>
       </c>
       <c r="AE46">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1.0315652859815827</v>
       </c>
     </row>
     <row r="47" spans="3:31" ht="18" thickBot="1">
       <c r="C47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2018</v>
       </c>
       <c r="D47" s="3">
@@ -8963,13 +8968,13 @@
         <v>2.1</v>
       </c>
       <c r="AE47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1.0529130131709286</v>
       </c>
     </row>
     <row r="48" spans="3:31" ht="18" thickBot="1">
       <c r="C48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2018</v>
       </c>
       <c r="D48" s="3">
@@ -9042,13 +9047,13 @@
         <v>1.5</v>
       </c>
       <c r="AE48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1.0683356568954763</v>
       </c>
     </row>
     <row r="49" spans="3:31" ht="18" thickBot="1">
       <c r="C49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2018</v>
       </c>
       <c r="D49" s="3">
@@ -9121,13 +9126,13 @@
         <v>1.6</v>
       </c>
       <c r="AE49">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1.0856660674322192</v>
       </c>
     </row>
     <row r="50" spans="3:31" ht="18" thickBot="1">
       <c r="C50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2018</v>
       </c>
       <c r="D50" s="3">
@@ -9200,13 +9205,13 @@
         <v>0.1</v>
       </c>
       <c r="AE50">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1.0869547272260336</v>
       </c>
     </row>
     <row r="51" spans="3:31" ht="18" thickBot="1">
       <c r="C51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2018</v>
       </c>
       <c r="D51" s="3">
@@ -9279,13 +9284,13 @@
         <v>1.3</v>
       </c>
       <c r="AE51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1.1006668011886855</v>
       </c>
     </row>
     <row r="52" spans="3:31" ht="18" thickBot="1">
       <c r="C52">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2018</v>
       </c>
       <c r="D52" s="3">
@@ -9358,13 +9363,13 @@
         <v>2.1</v>
       </c>
       <c r="AE52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1.1241149062626115</v>
       </c>
     </row>
     <row r="53" spans="3:31" ht="18" thickBot="1">
       <c r="C53">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2018</v>
       </c>
       <c r="D53" s="3">
@@ -9437,13 +9442,13 @@
         <v>2.4</v>
       </c>
       <c r="AE53">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1.1515711560333124</v>
       </c>
     </row>
     <row r="54" spans="3:31" ht="18" thickBot="1">
       <c r="C54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2018</v>
       </c>
       <c r="D54" s="3">
@@ -9516,13 +9521,13 @@
         <v>1.8</v>
       </c>
       <c r="AE54">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1.1724373555416956</v>
       </c>
     </row>
     <row r="55" spans="3:31" ht="18" thickBot="1">
       <c r="C55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2018</v>
       </c>
       <c r="D55" s="3">
@@ -9595,13 +9600,13 @@
         <v>1.2</v>
       </c>
       <c r="AE55">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>1.1869015298822319</v>
       </c>
     </row>
     <row r="56" spans="3:31" ht="18" thickBot="1">
       <c r="C56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2018</v>
       </c>
       <c r="D56" s="3">
@@ -9628,7 +9633,7 @@
     </row>
     <row r="57" spans="3:31" ht="18" thickBot="1">
       <c r="C57">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2018</v>
       </c>
       <c r="D57" s="3">
@@ -9655,7 +9660,7 @@
     </row>
     <row r="58" spans="3:31" ht="18" thickBot="1">
       <c r="C58">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2017</v>
       </c>
       <c r="D58" s="3">
@@ -9682,7 +9687,7 @@
     </row>
     <row r="59" spans="3:31" ht="18" thickBot="1">
       <c r="C59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2017</v>
       </c>
       <c r="D59" s="3">
@@ -9709,7 +9714,7 @@
     </row>
     <row r="60" spans="3:31" ht="18" thickBot="1">
       <c r="C60">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2017</v>
       </c>
       <c r="D60" s="3">
@@ -9736,7 +9741,7 @@
     </row>
     <row r="61" spans="3:31" ht="18" thickBot="1">
       <c r="C61">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2017</v>
       </c>
       <c r="D61" s="3">
@@ -9763,7 +9768,7 @@
     </row>
     <row r="62" spans="3:31" ht="18" thickBot="1">
       <c r="C62">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2017</v>
       </c>
       <c r="D62" s="3">
@@ -9790,7 +9795,7 @@
     </row>
     <row r="63" spans="3:31" ht="18" thickBot="1">
       <c r="C63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2017</v>
       </c>
       <c r="D63" s="3">
@@ -9817,7 +9822,7 @@
     </row>
     <row r="64" spans="3:31" ht="18" thickBot="1">
       <c r="C64">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2017</v>
       </c>
       <c r="D64" s="3">
@@ -9844,7 +9849,7 @@
     </row>
     <row r="65" spans="3:10" ht="18" thickBot="1">
       <c r="C65">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2017</v>
       </c>
       <c r="D65" s="3">
@@ -9871,7 +9876,7 @@
     </row>
     <row r="66" spans="3:10" ht="18" thickBot="1">
       <c r="C66">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2017</v>
       </c>
       <c r="D66" s="3">
@@ -9898,7 +9903,7 @@
     </row>
     <row r="67" spans="3:10" ht="18" thickBot="1">
       <c r="C67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2017</v>
       </c>
       <c r="D67" s="3">
@@ -9925,7 +9930,7 @@
     </row>
     <row r="68" spans="3:10" ht="18" thickBot="1">
       <c r="C68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2017</v>
       </c>
       <c r="D68" s="3">
@@ -9952,7 +9957,7 @@
     </row>
     <row r="69" spans="3:10" ht="18" thickBot="1">
       <c r="C69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2017</v>
       </c>
       <c r="D69" s="3">
@@ -9979,7 +9984,7 @@
     </row>
     <row r="70" spans="3:10" ht="18" thickBot="1">
       <c r="C70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2016</v>
       </c>
       <c r="D70" s="3">
@@ -10006,7 +10011,7 @@
     </row>
     <row r="71" spans="3:10" ht="18" thickBot="1">
       <c r="C71">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2016</v>
       </c>
       <c r="D71" s="3">
@@ -10033,7 +10038,7 @@
     </row>
     <row r="72" spans="3:10" ht="18" thickBot="1">
       <c r="C72">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2016</v>
       </c>
       <c r="D72" s="3">
@@ -10060,7 +10065,7 @@
     </row>
     <row r="73" spans="3:10" ht="18" thickBot="1">
       <c r="C73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2016</v>
       </c>
       <c r="D73" s="3">
@@ -10087,7 +10092,7 @@
     </row>
     <row r="74" spans="3:10" ht="18" thickBot="1">
       <c r="C74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2016</v>
       </c>
       <c r="D74" s="3">
@@ -10114,7 +10119,7 @@
     </row>
     <row r="75" spans="3:10" ht="18" thickBot="1">
       <c r="C75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2016</v>
       </c>
       <c r="D75" s="3">
@@ -10141,7 +10146,7 @@
     </row>
     <row r="76" spans="3:10" ht="18" thickBot="1">
       <c r="C76">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2016</v>
       </c>
       <c r="D76" s="3">
@@ -10168,7 +10173,7 @@
     </row>
     <row r="77" spans="3:10" ht="18" thickBot="1">
       <c r="C77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2016</v>
       </c>
       <c r="D77" s="3">
@@ -10195,7 +10200,7 @@
     </row>
     <row r="78" spans="3:10" ht="18" thickBot="1">
       <c r="C78">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2016</v>
       </c>
       <c r="D78" s="3">
@@ -10222,7 +10227,7 @@
     </row>
     <row r="79" spans="3:10" ht="18" thickBot="1">
       <c r="C79">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2016</v>
       </c>
       <c r="D79" s="3">
@@ -10249,7 +10254,7 @@
     </row>
     <row r="80" spans="3:10" ht="18" thickBot="1">
       <c r="C80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2016</v>
       </c>
       <c r="D80" s="3">
@@ -10276,7 +10281,7 @@
     </row>
     <row r="81" spans="3:10" ht="18" thickBot="1">
       <c r="C81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2016</v>
       </c>
       <c r="D81" s="3">
@@ -10303,7 +10308,7 @@
     </row>
     <row r="82" spans="3:10" ht="18" thickBot="1">
       <c r="C82">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2015</v>
       </c>
       <c r="D82" s="3">
@@ -10330,7 +10335,7 @@
     </row>
     <row r="83" spans="3:10" ht="18" thickBot="1">
       <c r="C83">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2015</v>
       </c>
       <c r="D83" s="3">
@@ -10357,7 +10362,7 @@
     </row>
     <row r="84" spans="3:10" ht="18" thickBot="1">
       <c r="C84">
-        <f t="shared" ref="C84:C147" si="8">YEAR(D84)</f>
+        <f t="shared" ref="C84:C147" si="11">YEAR(D84)</f>
         <v>2015</v>
       </c>
       <c r="D84" s="3">
@@ -10384,7 +10389,7 @@
     </row>
     <row r="85" spans="3:10" ht="18" thickBot="1">
       <c r="C85">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2015</v>
       </c>
       <c r="D85" s="3">
@@ -10411,7 +10416,7 @@
     </row>
     <row r="86" spans="3:10" ht="18" thickBot="1">
       <c r="C86">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2015</v>
       </c>
       <c r="D86" s="3">
@@ -10438,7 +10443,7 @@
     </row>
     <row r="87" spans="3:10" ht="18" thickBot="1">
       <c r="C87">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2015</v>
       </c>
       <c r="D87" s="3">
@@ -10465,7 +10470,7 @@
     </row>
     <row r="88" spans="3:10" ht="18" thickBot="1">
       <c r="C88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2015</v>
       </c>
       <c r="D88" s="3">
@@ -10492,7 +10497,7 @@
     </row>
     <row r="89" spans="3:10" ht="18" thickBot="1">
       <c r="C89">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2015</v>
       </c>
       <c r="D89" s="3">
@@ -10519,7 +10524,7 @@
     </row>
     <row r="90" spans="3:10" ht="18" thickBot="1">
       <c r="C90">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2015</v>
       </c>
       <c r="D90" s="3">
@@ -10546,7 +10551,7 @@
     </row>
     <row r="91" spans="3:10" ht="18" thickBot="1">
       <c r="C91">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2015</v>
       </c>
       <c r="D91" s="3">
@@ -10573,7 +10578,7 @@
     </row>
     <row r="92" spans="3:10" ht="18" thickBot="1">
       <c r="C92">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2015</v>
       </c>
       <c r="D92" s="3">
@@ -10600,7 +10605,7 @@
     </row>
     <row r="93" spans="3:10" ht="18" thickBot="1">
       <c r="C93">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2015</v>
       </c>
       <c r="D93" s="3">
@@ -10627,7 +10632,7 @@
     </row>
     <row r="94" spans="3:10" ht="18" thickBot="1">
       <c r="C94">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2014</v>
       </c>
       <c r="D94" s="3">
@@ -10654,7 +10659,7 @@
     </row>
     <row r="95" spans="3:10" ht="18" thickBot="1">
       <c r="C95">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2014</v>
       </c>
       <c r="D95" s="3">
@@ -10681,7 +10686,7 @@
     </row>
     <row r="96" spans="3:10" ht="18" thickBot="1">
       <c r="C96">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2014</v>
       </c>
       <c r="D96" s="3">
@@ -10708,7 +10713,7 @@
     </row>
     <row r="97" spans="3:10" ht="18" thickBot="1">
       <c r="C97">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2014</v>
       </c>
       <c r="D97" s="3">
@@ -10735,7 +10740,7 @@
     </row>
     <row r="98" spans="3:10" ht="18" thickBot="1">
       <c r="C98">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2014</v>
       </c>
       <c r="D98" s="3">
@@ -10762,7 +10767,7 @@
     </row>
     <row r="99" spans="3:10" ht="18" thickBot="1">
       <c r="C99">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2014</v>
       </c>
       <c r="D99" s="3">
@@ -10789,7 +10794,7 @@
     </row>
     <row r="100" spans="3:10" ht="18" thickBot="1">
       <c r="C100">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2014</v>
       </c>
       <c r="D100" s="3">
@@ -10816,7 +10821,7 @@
     </row>
     <row r="101" spans="3:10" ht="18" thickBot="1">
       <c r="C101">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2014</v>
       </c>
       <c r="D101" s="3">
@@ -10843,7 +10848,7 @@
     </row>
     <row r="102" spans="3:10" ht="18" thickBot="1">
       <c r="C102">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2014</v>
       </c>
       <c r="D102" s="3">
@@ -10870,7 +10875,7 @@
     </row>
     <row r="103" spans="3:10" ht="18" thickBot="1">
       <c r="C103">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2014</v>
       </c>
       <c r="D103" s="3">
@@ -10897,7 +10902,7 @@
     </row>
     <row r="104" spans="3:10" ht="18" thickBot="1">
       <c r="C104">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2014</v>
       </c>
       <c r="D104" s="3">
@@ -10924,7 +10929,7 @@
     </row>
     <row r="105" spans="3:10" ht="18" thickBot="1">
       <c r="C105">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2014</v>
       </c>
       <c r="D105" s="3">
@@ -10951,7 +10956,7 @@
     </row>
     <row r="106" spans="3:10" ht="18" thickBot="1">
       <c r="C106">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2013</v>
       </c>
       <c r="D106" s="3">
@@ -10978,7 +10983,7 @@
     </row>
     <row r="107" spans="3:10" ht="18" thickBot="1">
       <c r="C107">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2013</v>
       </c>
       <c r="D107" s="3">
@@ -11005,7 +11010,7 @@
     </row>
     <row r="108" spans="3:10" ht="18" thickBot="1">
       <c r="C108">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2013</v>
       </c>
       <c r="D108" s="3">
@@ -11032,7 +11037,7 @@
     </row>
     <row r="109" spans="3:10" ht="18" thickBot="1">
       <c r="C109">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2013</v>
       </c>
       <c r="D109" s="3">
@@ -11059,7 +11064,7 @@
     </row>
     <row r="110" spans="3:10" ht="18" thickBot="1">
       <c r="C110">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2013</v>
       </c>
       <c r="D110" s="3">
@@ -11086,7 +11091,7 @@
     </row>
     <row r="111" spans="3:10" ht="18" thickBot="1">
       <c r="C111">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2013</v>
       </c>
       <c r="D111" s="3">
@@ -11113,7 +11118,7 @@
     </row>
     <row r="112" spans="3:10" ht="18" thickBot="1">
       <c r="C112">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2013</v>
       </c>
       <c r="D112" s="3">
@@ -11140,7 +11145,7 @@
     </row>
     <row r="113" spans="3:10" ht="18" thickBot="1">
       <c r="C113">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2013</v>
       </c>
       <c r="D113" s="3">
@@ -11167,7 +11172,7 @@
     </row>
     <row r="114" spans="3:10" ht="18" thickBot="1">
       <c r="C114">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2013</v>
       </c>
       <c r="D114" s="3">
@@ -11194,7 +11199,7 @@
     </row>
     <row r="115" spans="3:10" ht="18" thickBot="1">
       <c r="C115">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2013</v>
       </c>
       <c r="D115" s="3">
@@ -11221,7 +11226,7 @@
     </row>
     <row r="116" spans="3:10" ht="18" thickBot="1">
       <c r="C116">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2013</v>
       </c>
       <c r="D116" s="3">
@@ -11248,7 +11253,7 @@
     </row>
     <row r="117" spans="3:10" ht="18" thickBot="1">
       <c r="C117">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2013</v>
       </c>
       <c r="D117" s="3">
@@ -11275,7 +11280,7 @@
     </row>
     <row r="118" spans="3:10" ht="18" thickBot="1">
       <c r="C118">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2012</v>
       </c>
       <c r="D118" s="3">
@@ -11302,7 +11307,7 @@
     </row>
     <row r="119" spans="3:10" ht="18" thickBot="1">
       <c r="C119">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2012</v>
       </c>
       <c r="D119" s="3">
@@ -11329,7 +11334,7 @@
     </row>
     <row r="120" spans="3:10" ht="18" thickBot="1">
       <c r="C120">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2012</v>
       </c>
       <c r="D120" s="3">
@@ -11356,7 +11361,7 @@
     </row>
     <row r="121" spans="3:10" ht="18" thickBot="1">
       <c r="C121">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2012</v>
       </c>
       <c r="D121" s="3">
@@ -11383,7 +11388,7 @@
     </row>
     <row r="122" spans="3:10" ht="18" thickBot="1">
       <c r="C122">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2012</v>
       </c>
       <c r="D122" s="3">
@@ -11410,7 +11415,7 @@
     </row>
     <row r="123" spans="3:10" ht="18" thickBot="1">
       <c r="C123">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2012</v>
       </c>
       <c r="D123" s="3">
@@ -11437,7 +11442,7 @@
     </row>
     <row r="124" spans="3:10" ht="18" thickBot="1">
       <c r="C124">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2012</v>
       </c>
       <c r="D124" s="3">
@@ -11464,7 +11469,7 @@
     </row>
     <row r="125" spans="3:10" ht="18" thickBot="1">
       <c r="C125">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2012</v>
       </c>
       <c r="D125" s="3">
@@ -11491,7 +11496,7 @@
     </row>
     <row r="126" spans="3:10" ht="18" thickBot="1">
       <c r="C126">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2012</v>
       </c>
       <c r="D126" s="3">
@@ -11518,7 +11523,7 @@
     </row>
     <row r="127" spans="3:10" ht="18" thickBot="1">
       <c r="C127">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2012</v>
       </c>
       <c r="D127" s="3">
@@ -11545,7 +11550,7 @@
     </row>
     <row r="128" spans="3:10" ht="18" thickBot="1">
       <c r="C128">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2012</v>
       </c>
       <c r="D128" s="3">
@@ -11572,7 +11577,7 @@
     </row>
     <row r="129" spans="3:10" ht="18" thickBot="1">
       <c r="C129">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2012</v>
       </c>
       <c r="D129" s="3">
@@ -11599,7 +11604,7 @@
     </row>
     <row r="130" spans="3:10" ht="18" thickBot="1">
       <c r="C130">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2011</v>
       </c>
       <c r="D130" s="3">
@@ -11626,7 +11631,7 @@
     </row>
     <row r="131" spans="3:10" ht="18" thickBot="1">
       <c r="C131">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2011</v>
       </c>
       <c r="D131" s="3">
@@ -11653,7 +11658,7 @@
     </row>
     <row r="132" spans="3:10" ht="18" thickBot="1">
       <c r="C132">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2011</v>
       </c>
       <c r="D132" s="3">
@@ -11680,7 +11685,7 @@
     </row>
     <row r="133" spans="3:10" ht="18" thickBot="1">
       <c r="C133">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2011</v>
       </c>
       <c r="D133" s="3">
@@ -11707,7 +11712,7 @@
     </row>
     <row r="134" spans="3:10" ht="18" thickBot="1">
       <c r="C134">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2011</v>
       </c>
       <c r="D134" s="3">
@@ -11734,7 +11739,7 @@
     </row>
     <row r="135" spans="3:10" ht="18" thickBot="1">
       <c r="C135">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2011</v>
       </c>
       <c r="D135" s="3">
@@ -11761,7 +11766,7 @@
     </row>
     <row r="136" spans="3:10" ht="18" thickBot="1">
       <c r="C136">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2011</v>
       </c>
       <c r="D136" s="3">
@@ -11788,7 +11793,7 @@
     </row>
     <row r="137" spans="3:10" ht="18" thickBot="1">
       <c r="C137">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2011</v>
       </c>
       <c r="D137" s="3">
@@ -11815,7 +11820,7 @@
     </row>
     <row r="138" spans="3:10" ht="18" thickBot="1">
       <c r="C138">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2011</v>
       </c>
       <c r="D138" s="3">
@@ -11842,7 +11847,7 @@
     </row>
     <row r="139" spans="3:10" ht="18" thickBot="1">
       <c r="C139">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2011</v>
       </c>
       <c r="D139" s="3">
@@ -11869,7 +11874,7 @@
     </row>
     <row r="140" spans="3:10" ht="18" thickBot="1">
       <c r="C140">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2011</v>
       </c>
       <c r="D140" s="3">
@@ -11896,7 +11901,7 @@
     </row>
     <row r="141" spans="3:10" ht="18" thickBot="1">
       <c r="C141">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2011</v>
       </c>
       <c r="D141" s="3">
@@ -11923,7 +11928,7 @@
     </row>
     <row r="142" spans="3:10" ht="18" thickBot="1">
       <c r="C142">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2010</v>
       </c>
       <c r="D142" s="3">
@@ -11950,7 +11955,7 @@
     </row>
     <row r="143" spans="3:10" ht="18" thickBot="1">
       <c r="C143">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2010</v>
       </c>
       <c r="D143" s="3">
@@ -11977,7 +11982,7 @@
     </row>
     <row r="144" spans="3:10" ht="18" thickBot="1">
       <c r="C144">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2010</v>
       </c>
       <c r="D144" s="3">
@@ -12004,7 +12009,7 @@
     </row>
     <row r="145" spans="3:10" ht="18" thickBot="1">
       <c r="C145">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2010</v>
       </c>
       <c r="D145" s="3">
@@ -12031,7 +12036,7 @@
     </row>
     <row r="146" spans="3:10" ht="18" thickBot="1">
       <c r="C146">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2010</v>
       </c>
       <c r="D146" s="3">
@@ -12058,7 +12063,7 @@
     </row>
     <row r="147" spans="3:10" ht="18" thickBot="1">
       <c r="C147">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2010</v>
       </c>
       <c r="D147" s="3">
@@ -12085,7 +12090,7 @@
     </row>
     <row r="148" spans="3:10" ht="18" thickBot="1">
       <c r="C148">
-        <f t="shared" ref="C148:C153" si="9">YEAR(D148)</f>
+        <f t="shared" ref="C148:C153" si="12">YEAR(D148)</f>
         <v>2010</v>
       </c>
       <c r="D148" s="3">
@@ -12112,7 +12117,7 @@
     </row>
     <row r="149" spans="3:10" ht="18" thickBot="1">
       <c r="C149">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2010</v>
       </c>
       <c r="D149" s="3">
@@ -12139,7 +12144,7 @@
     </row>
     <row r="150" spans="3:10" ht="18" thickBot="1">
       <c r="C150">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2010</v>
       </c>
       <c r="D150" s="3">
@@ -12166,7 +12171,7 @@
     </row>
     <row r="151" spans="3:10" ht="18" thickBot="1">
       <c r="C151">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2010</v>
       </c>
       <c r="D151" s="3">
@@ -12193,7 +12198,7 @@
     </row>
     <row r="152" spans="3:10" ht="18" thickBot="1">
       <c r="C152">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2010</v>
       </c>
       <c r="D152" s="3">
@@ -12220,7 +12225,7 @@
     </row>
     <row r="153" spans="3:10" ht="17.25">
       <c r="C153">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2010</v>
       </c>
       <c r="D153" s="9">
@@ -12253,6 +12258,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D065B385-3D13-43B2-889B-99806AF0521A}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A3:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>